<commit_message>
add more keyword driven: iFrame, Select
</commit_message>
<xml_diff>
--- a/out/production/KeyWordDriven/testing/dataEngine/TestSuite1.xlsx
+++ b/out/production/KeyWordDriven/testing/dataEngine/TestSuite1.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="2" r:id="rId1"/>
     <sheet name="TestCase1" sheetId="1" r:id="rId2"/>
     <sheet name="TestCase2" sheetId="4" r:id="rId3"/>
     <sheet name="TestCase3" sheetId="5" r:id="rId4"/>
+    <sheet name="TestCase4" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="89">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -240,9 +241,6 @@
     <t>navigateToBack</t>
   </si>
   <si>
-    <t>waitAndPause</t>
-  </si>
-  <si>
     <t>openBrowser</t>
   </si>
   <si>
@@ -250,6 +248,48 @@
   </si>
   <si>
     <t>TXT_LEADERSHIP</t>
+  </si>
+  <si>
+    <t>verifyElementIsExisted</t>
+  </si>
+  <si>
+    <t>TS_008</t>
+  </si>
+  <si>
+    <t>Verify text</t>
+  </si>
+  <si>
+    <t>verifyText</t>
+  </si>
+  <si>
+    <t>TXT_AGILETESTING</t>
+  </si>
+  <si>
+    <t>Agile Testing and ATDD Automation –  Free Tutorials</t>
+  </si>
+  <si>
+    <t>http://toolsqa.wpengine.com/iframe-practice-page/</t>
+  </si>
+  <si>
+    <t>Go to Practiceform page to do switch iFrame</t>
+  </si>
+  <si>
+    <t>switchToIFrameWithName</t>
+  </si>
+  <si>
+    <t>iframe1</t>
+  </si>
+  <si>
+    <t>Wait</t>
+  </si>
+  <si>
+    <t>iFrame example</t>
+  </si>
+  <si>
+    <t>switchToMainPage</t>
+  </si>
+  <si>
+    <t>Go to home page frame</t>
   </si>
 </sst>
 </file>
@@ -445,14 +485,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -996,13 +1036,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2579,8 +2619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,8 +2664,8 @@
       <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
+      <c r="C2" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="D2" s="3"/>
       <c r="G2" s="12" t="s">
@@ -2633,20 +2673,20 @@
       </c>
       <c r="H2" s="13">
         <f>SUM(H3:H4)</f>
-        <v>9</v>
-      </c>
-      <c r="I2" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="19">
+      <c r="J2" s="18">
         <f>SUM(J3:J4)</f>
         <v>0</v>
       </c>
       <c r="K2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="17">
-        <f>(J2/H2)*100</f>
+      <c r="L2" s="19">
+        <f>(J2/H2)</f>
         <v>0</v>
       </c>
     </row>
@@ -2668,18 +2708,18 @@
         <f>COUNTIF(C2:C44,"Yes")</f>
         <v>1</v>
       </c>
-      <c r="I3" s="18" t="s">
+      <c r="I3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="18">
         <f>COUNTIF($D2:$D4,"PASSED")</f>
         <v>0</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="L3" s="17" t="e">
-        <f>(J3/J2)*100</f>
+      <c r="L3" s="19" t="e">
+        <f>(J3/J2)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2699,20 +2739,20 @@
       </c>
       <c r="H4" s="13">
         <f>COUNTIF(C3:C45,"No")</f>
-        <v>8</v>
-      </c>
-      <c r="I4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="18">
         <f>COUNTIF($D2:$D4,"FAILED")</f>
         <v>0</v>
       </c>
       <c r="K4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="17" t="e">
-        <f>(J4/J2)*100</f>
+      <c r="L4" s="19" t="e">
+        <f>(J4/J2)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -2721,10 +2761,10 @@
         <v>55</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>57</v>
+        <v>86</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D5" s="2"/>
     </row>
@@ -2800,10 +2840,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2850,7 +2890,7 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>25</v>
@@ -2917,10 +2957,10 @@
         <v>65</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -2934,9 +2974,11 @@
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E7" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F7" s="7"/>
     </row>
@@ -2948,13 +2990,33 @@
         <v>67</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3014,7 +3076,7 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" s="2"/>
     </row>
@@ -3124,7 +3186,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3171,7 +3233,7 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>35</v>
@@ -3255,4 +3317,170 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="49.140625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F5" r:id="rId2" display="doai.tran@seldatinc.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add more testcases for some keyword
</commit_message>
<xml_diff>
--- a/out/production/KeyWordDriven/testing/dataEngine/TestSuite1.xlsx
+++ b/out/production/KeyWordDriven/testing/dataEngine/TestSuite1.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="97">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Wait 5000 mls</t>
   </si>
   <si>
-    <t>waitandPause</t>
-  </si>
-  <si>
     <t>Page objects</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>send some value to textbox</t>
   </si>
   <si>
-    <t>input</t>
-  </si>
-  <si>
     <t>ABCDEDF GHYUI IOPU</t>
   </si>
   <si>
@@ -289,7 +283,37 @@
     <t>switchToMainPage</t>
   </si>
   <si>
-    <t>Go to home page frame</t>
+    <t>TS_009</t>
+  </si>
+  <si>
+    <t>switchToIFrameWithID</t>
+  </si>
+  <si>
+    <t>IF1</t>
+  </si>
+  <si>
+    <t>Switch to iFrame using Name</t>
+  </si>
+  <si>
+    <t>Switch to iFrame using iframe ID</t>
+  </si>
+  <si>
+    <t>Swith to home page iframe</t>
+  </si>
+  <si>
+    <t>Menu and hover example</t>
+  </si>
+  <si>
+    <t>WMB_TUTORIALS</t>
+  </si>
+  <si>
+    <t>moveToElement</t>
+  </si>
+  <si>
+    <t>WMB_STRATEGICDECISION</t>
+  </si>
+  <si>
+    <t>waitAndPause</t>
   </si>
 </sst>
 </file>
@@ -1039,10 +1063,10 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2619,8 +2643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2637,19 +2661,19 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H1" s="21"/>
       <c r="I1" s="21"/>
@@ -2659,31 +2683,31 @@
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D2" s="3"/>
       <c r="G2" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H2" s="13">
         <f>SUM(H3:H4)</f>
         <v>8</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J2" s="18">
         <f>SUM(J3:J4)</f>
         <v>0</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L2" s="19">
         <f>(J2/H2)</f>
@@ -2692,31 +2716,31 @@
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" s="3"/>
       <c r="G3" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H3" s="13">
         <f>COUNTIF(C2:C44,"Yes")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J3" s="18">
         <f>COUNTIF($D2:$D4,"PASSED")</f>
         <v>0</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L3" s="19" t="e">
         <f>(J3/J2)</f>
@@ -2725,31 +2749,31 @@
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>57</v>
+        <v>92</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D4" s="3"/>
       <c r="G4" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H4" s="13">
         <f>COUNTIF(C3:C45,"No")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J4" s="18">
         <f>COUNTIF($D2:$D4,"FAILED")</f>
         <v>0</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L4" s="19" t="e">
         <f>(J4/J2)</f>
@@ -2758,73 +2782,73 @@
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D10" s="2"/>
     </row>
@@ -2843,7 +2867,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2866,21 +2890,21 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -2890,40 +2914,40 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>13</v>
@@ -2932,82 +2956,82 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="E8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>11</v>
@@ -3052,21 +3076,21 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -3076,80 +3100,80 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>52</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>13</v>
@@ -3158,10 +3182,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>11</v>
@@ -3183,10 +3207,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3209,21 +3233,21 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -3233,69 +3257,71 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
@@ -3303,11 +3329,73 @@
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="E6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F10" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3321,10 +3409,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3347,21 +3435,21 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -3371,33 +3459,33 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -3405,75 +3493,109 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>33</v>
+        <v>89</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F10" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Edit summary report on Excel and improve SetCellValue in Excel
</commit_message>
<xml_diff>
--- a/out/production/KeyWordDriven/testing/dataEngine/TestSuite1.xlsx
+++ b/out/production/KeyWordDriven/testing/dataEngine/TestSuite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="2" r:id="rId1"/>
@@ -12,7 +12,13 @@
     <sheet name="TestCase2" sheetId="4" r:id="rId3"/>
     <sheet name="TestCase3" sheetId="5" r:id="rId4"/>
     <sheet name="TestCase4" sheetId="6" r:id="rId5"/>
+    <sheet name="TestCase5" sheetId="7" r:id="rId6"/>
+    <sheet name="TestCase6" sheetId="8" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestSuite!$G$21:$G$22</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="0">TestSuite!$D$2</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="128">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -88,9 +94,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Test Link on Home Page</t>
-  </si>
-  <si>
     <t>Click to Link</t>
   </si>
   <si>
@@ -136,9 +139,6 @@
     <t>TestCase3</t>
   </si>
   <si>
-    <t>Sumary Report</t>
-  </si>
-  <si>
     <t>Total of test cases</t>
   </si>
   <si>
@@ -314,6 +314,105 @@
   </si>
   <si>
     <t>waitAndPause</t>
+  </si>
+  <si>
+    <t>PASSED</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>Home Page and verified elements</t>
+  </si>
+  <si>
+    <t>Practiceform page - TextBox, Select Box</t>
+  </si>
+  <si>
+    <t>selectByVisibleText</t>
+  </si>
+  <si>
+    <t>Select option 1 on Select option</t>
+  </si>
+  <si>
+    <t>Select option 2 on Select option</t>
+  </si>
+  <si>
+    <t>LST_OPTION</t>
+  </si>
+  <si>
+    <t>Option 1</t>
+  </si>
+  <si>
+    <t>Option 2</t>
+  </si>
+  <si>
+    <t>Click option 1 on Radio</t>
+  </si>
+  <si>
+    <t>LBL_OPTION1</t>
+  </si>
+  <si>
+    <t>Close Browser</t>
+  </si>
+  <si>
+    <t>Go to Practice form site</t>
+  </si>
+  <si>
+    <t>Select a date form.</t>
+  </si>
+  <si>
+    <t>Click on date form</t>
+  </si>
+  <si>
+    <t>TEXT_DATE</t>
+  </si>
+  <si>
+    <t>Click to adjust to + 1 month</t>
+  </si>
+  <si>
+    <t>BTN_ADDMONTH</t>
+  </si>
+  <si>
+    <t>Click to adjust to - 1 month</t>
+  </si>
+  <si>
+    <t>BTN_SWBMONTH</t>
+  </si>
+  <si>
+    <t>TBL_DAY22</t>
+  </si>
+  <si>
+    <t>%Not Yet</t>
+  </si>
+  <si>
+    <t>Passed - Failed</t>
+  </si>
+  <si>
+    <t>Summary Report</t>
+  </si>
+  <si>
+    <t>Executed Summary</t>
+  </si>
+  <si>
+    <t>11/23/2016</t>
+  </si>
+  <si>
+    <t>ybox.com</t>
+  </si>
+  <si>
+    <t>TXT_URL</t>
+  </si>
+  <si>
+    <t>TEXT_URLERROR</t>
+  </si>
+  <si>
+    <t>Please enter a valid URL.</t>
+  </si>
+  <si>
+    <t>http://www.seleniumframework.com</t>
+  </si>
+  <si>
+    <t>submit</t>
   </si>
 </sst>
 </file>
@@ -365,7 +464,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -402,8 +501,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="31"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -455,7 +560,9 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -463,11 +570,24 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -475,7 +595,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -492,7 +612,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -518,12 +637,33 @@
     <xf numFmtId="10" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -531,6 +671,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -563,9 +708,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="50" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -574,7 +722,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Passed / Failed</a:t>
+              <a:t>PASSED - FAILED</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -592,9 +740,12 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="50" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -617,36 +768,23 @@
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent1">
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent1">
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent1">
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
               <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -658,36 +796,23 @@
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
             <c:spPr>
-              <a:gradFill rotWithShape="1">
-                <a:gsLst>
-                  <a:gs pos="0">
-                    <a:schemeClr val="accent2">
-                      <a:satMod val="103000"/>
-                      <a:lumMod val="102000"/>
-                      <a:tint val="94000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="50000">
-                    <a:schemeClr val="accent2">
-                      <a:satMod val="110000"/>
-                      <a:lumMod val="100000"/>
-                      <a:shade val="100000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="accent2">
-                      <a:lumMod val="99000"/>
-                      <a:satMod val="120000"/>
-                      <a:shade val="78000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
               <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -710,9 +835,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:schemeClr val="lt1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -722,7 +847,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="ctr"/>
+            <c:dLblPos val="inEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -732,13 +857,14 @@
             <c:showLeaderLines val="1"/>
             <c:leaderLines>
               <c:spPr>
-                <a:ln w="9525">
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                   <a:solidFill>
-                    <a:schemeClr val="tx2">
+                    <a:schemeClr val="tx1">
                       <a:lumMod val="35000"/>
                       <a:lumOff val="65000"/>
                     </a:schemeClr>
                   </a:solidFill>
+                  <a:round/>
                 </a:ln>
                 <a:effectLst/>
               </c:spPr>
@@ -800,7 +926,7 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
+          <c:dLblPos val="inEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -820,7 +946,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -836,7 +962,10 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -857,7 +986,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx2">
+        <a:schemeClr val="tx1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -905,7 +1034,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -919,16 +1048,24 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" b="1"/>
-              <a:t>Test</a:t>
+              <a:t>TESTCASE</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" b="1" baseline="0"/>
-              <a:t>Case Execution</a:t>
+              <a:t> SUMMARY</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.23675728316765834"/>
+          <c:y val="2.8673824335572549E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -942,7 +1079,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -968,11 +1105,7 @@
     <c:floor>
       <c:thickness val="0"/>
       <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="27000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:noFill/>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -1016,24 +1149,10 @@
               <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
-            <a:scene3d>
-              <a:camera prst="orthographicFront"/>
-              <a:lightRig rig="threePt" dir="t"/>
-            </a:scene3d>
-            <a:sp3d prstMaterial="translucentPowder">
-              <a:contourClr>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:contourClr>
-            </a:sp3d>
+            <a:sp3d/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
@@ -1063,10 +1182,10 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1117,8 +1236,8 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1148,8 +1267,8 @@
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1176,8 +1295,8 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
-                    <a:lumMod val="50000"/>
-                    <a:lumOff val="50000"/>
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1200,6 +1319,322 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="50" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Executed Summary</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14132217213264567"/>
+          <c:y val="3.8231780167264036E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="50" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:doughnutChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-1715-4962-B384-21601D87ECE4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+              <a:scene3d>
+                <a:camera prst="orthographicFront"/>
+                <a:lightRig rig="brightRoom" dir="t"/>
+              </a:scene3d>
+              <a:sp3d prstMaterial="flat">
+                <a:bevelT w="50800" h="101600" prst="angle"/>
+                <a:contourClr>
+                  <a:srgbClr val="000000"/>
+                </a:contourClr>
+              </a:sp3d>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1715-4962-B384-21601D87ECE4}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="35000"/>
+                      <a:lumOff val="65000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:round/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>TestSuite!$M$3:$M$4</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>%Total executed</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>%Not Yet</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TestSuite!$N$3:$N$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1715-4962-B384-21601D87ECE4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+        <c:holeSize val="50"/>
+      </c:doughnutChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1317,484 +1752,56 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="255">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk2">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="31750" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="3">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="12700">
-        <a:solidFill>
-          <a:schemeClr val="lt2"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="3"/>
-    <cs:effectRef idx="2"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="60000"/>
-            <a:lumOff val="40000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="dash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="1600" b="1" kern="1200"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDash"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx2"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="292">
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1805,8 +1812,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1832,19 +1839,16 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -1875,9 +1879,7 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
+    <cs:lnRef idx="0"/>
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
@@ -1889,19 +1891,20 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="brightRoom" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="flat">
+        <a:bevelT w="50800" h="101600" prst="angle"/>
+        <a:contourClr>
+          <a:srgbClr val="000000"/>
+        </a:contourClr>
+      </a:sp3d>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
+    <cs:lnRef idx="0"/>
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
@@ -1913,18 +1916,11 @@
       <a:solidFill>
         <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln>
+      <a:ln w="19050">
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
+          <a:schemeClr val="lt1"/>
         </a:solidFill>
       </a:ln>
-      <a:scene3d>
-        <a:camera prst="orthographicFront"/>
-        <a:lightRig rig="threePt" dir="t"/>
-      </a:scene3d>
-      <a:sp3d prstMaterial="translucentPowder"/>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -1939,36 +1935,28 @@
     <cs:spPr>
       <a:ln w="28575" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="70000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
+    <cs:lnRef idx="0"/>
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="70000"/>
-        </a:schemeClr>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln>
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
+          <a:schemeClr val="lt1"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
@@ -1998,18 +1986,20 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2019,7 +2009,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -2028,13 +2018,14 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2043,10 +2034,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -2062,14 +2053,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2084,15 +2075,32 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:alpha val="27000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:sp3d/>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
     </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -2110,34 +2118,35 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -2147,24 +2156,6 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
   </cs:leaderLine>
   <cs:legend>
     <cs:lnRef idx="0"/>
@@ -2172,8 +2163,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2200,8 +2191,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2211,10 +2202,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -2235,7 +2226,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1600" b="0" kern="1200" cap="none" spc="50" baseline="0"/>
+    <cs:defRPr sz="1400" b="1" i="0" kern="1200" cap="all" spc="50" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2244,13 +2235,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="15875" cap="rnd">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2260,8 +2252,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2271,19 +2263,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2293,8 +2286,8 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2307,7 +2300,1021 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:sp3d/>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="258">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:scene3d>
+        <a:camera prst="orthographicFront"/>
+        <a:lightRig rig="brightRoom" dir="t"/>
+      </a:scene3d>
+      <a:sp3d prstMaterial="flat">
+        <a:bevelT w="50800" h="101600" prst="angle"/>
+        <a:contourClr>
+          <a:srgbClr val="000000"/>
+        </a:contourClr>
+      </a:sp3d>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" i="0" kern="1200" cap="all" spc="50" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
     </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
@@ -2317,16 +3324,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>257177</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>809625</xdr:colOff>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2347,16 +3354,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2370,6 +3377,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152401</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2641,7 +3678,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -2652,210 +3689,247 @@
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="40.140625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="4.28515625" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="8.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="7.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.28515625" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-    </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="G2" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="13">
+      <c r="G2" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="12">
         <f>SUM(H3:H4)</f>
         <v>8</v>
       </c>
-      <c r="I2" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="18">
+      <c r="I2" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="17">
         <f>SUM(J3:J4)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="19">
-        <f>(J2/H2)</f>
+      <c r="K2" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="L2" s="24"/>
+      <c r="M2" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="N2" s="26"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="G3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="12">
+        <f>COUNTIF(C2:C44,"Yes")</f>
+        <v>3</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="17">
+        <f>COUNTIF($D2:$D400,"PASSED")</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="G3" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="13">
-        <f>COUNTIF(C2:C44,"Yes")</f>
-        <v>2</v>
-      </c>
-      <c r="I3" s="17" t="s">
+      <c r="K3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="18">
-        <f>COUNTIF($D2:$D4,"PASSED")</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="19" t="e">
+      <c r="L3" s="18" t="e">
         <f>(J3/J2)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M3" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="21">
+        <f>J2/H2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>90</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="12">
+        <f>COUNTIF(C3:C45,"No")</f>
+        <v>5</v>
+      </c>
+      <c r="I4" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="13">
-        <f>COUNTIF(C3:C45,"No")</f>
-        <v>6</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" s="18">
-        <f>COUNTIF($D2:$D4,"FAILED")</f>
+      <c r="J4" s="17">
+        <f>COUNTIF($D2:$D400,"FAILED")</f>
         <v>0</v>
       </c>
-      <c r="K4" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" s="19" t="e">
+      <c r="K4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="18" t="e">
         <f>(J4/J2)</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M4" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="N4" s="21">
+        <f>1-N3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="B10" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="G1:L1"/>
+  <mergeCells count="3">
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="G1:N1"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10">
+      <formula1>$G$21:$G$22</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2864,7 +3938,212 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="49.140625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="I3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G9">
+      <formula1>$I$2:$I$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -2879,7 +4158,7 @@
     <col min="6" max="6" width="49.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2902,7 +4181,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -2914,47 +4193,58 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>61</v>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="2"/>
+      <c r="I3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -2962,15 +4252,20 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="E5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>34</v>
       </c>
@@ -2978,82 +4273,115 @@
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>105</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="E9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="2"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G7">
+      <formula1>$I$2:$I$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3065,7 +4393,7 @@
     <col min="6" max="6" width="49.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3088,7 +4416,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -3100,11 +4428,17 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
@@ -3112,102 +4446,381 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="I3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G10">
+      <formula1>$I$2:$I$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="49.140625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="I3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="C6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
+        <v>62</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G10">
+      <formula1>$I$2:$I$3</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F5" r:id="rId2" display="doai.tran@seldatinc.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
@@ -3222,7 +4835,7 @@
     <col min="6" max="6" width="49.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3245,9 +4858,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -3257,162 +4870,166 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="I3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="3" t="s">
+        <v>112</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>94</v>
+        <v>13</v>
       </c>
       <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="D7" s="2" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="2" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>72</v>
+      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>96</v>
+        <v>12</v>
       </c>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="2"/>
+      <c r="G9" s="2"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G9">
+      <formula1>$I$2:$I$3</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1"/>
-    <hyperlink ref="F4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3424,7 +5041,7 @@
     <col min="6" max="6" width="49.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3447,9 +5064,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -3459,148 +5076,157 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>80</v>
+        <v>108</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="I3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F4" s="8"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>123</v>
+      </c>
       <c r="E5" s="3" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="29"/>
+      <c r="D6" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>91</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>85</v>
+        <v>12</v>
       </c>
       <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="2"/>
+      <c r="G9" s="2"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6">
+      <formula1>$I$2:$I$3</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1"/>
-    <hyperlink ref="F5" r:id="rId2" display="doai.tran@seldatinc.com"/>
+    <hyperlink ref="F8" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>

</xml_diff>

<commit_message>
add keyword verifytextintable and testcase
</commit_message>
<xml_diff>
--- a/out/production/KeyWordDriven/testing/dataEngine/TestSuite1.xlsx
+++ b/out/production/KeyWordDriven/testing/dataEngine/TestSuite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="2" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="TestCase4" sheetId="6" r:id="rId5"/>
     <sheet name="TestCase5" sheetId="7" r:id="rId6"/>
     <sheet name="TestCase6" sheetId="8" r:id="rId7"/>
+    <sheet name="TestCase7" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestSuite!$G$21:$G$22</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="138">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -413,6 +414,36 @@
   </si>
   <si>
     <t>submit</t>
+  </si>
+  <si>
+    <t>Submit value after input</t>
+  </si>
+  <si>
+    <t>Verifytext value after input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inputvalue new value </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closebrowser </t>
+  </si>
+  <si>
+    <t>Input value on URL TextBox</t>
+  </si>
+  <si>
+    <t>http://only-testing-blog.blogspot.in/2013/11/new-test.html</t>
+  </si>
+  <si>
+    <t>wait</t>
+  </si>
+  <si>
+    <t>verifyTextInTable</t>
+  </si>
+  <si>
+    <t>TBL_TESTTABLE</t>
+  </si>
+  <si>
+    <t>22</t>
   </si>
 </sst>
 </file>
@@ -595,7 +626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -645,6 +676,8 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -663,7 +696,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1182,10 +1214,10 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3681,7 +3713,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3712,16 +3744,16 @@
       <c r="D1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -3748,14 +3780,14 @@
         <f>SUM(J3:J4)</f>
         <v>0</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="L2" s="24"/>
-      <c r="M2" s="25" t="s">
+      <c r="L2" s="26"/>
+      <c r="M2" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="N2" s="26"/>
+      <c r="N2" s="28"/>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3773,7 +3805,7 @@
       </c>
       <c r="H3" s="12">
         <f>COUNTIF(C2:C44,"Yes")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I3" s="16" t="s">
         <v>41</v>
@@ -3813,7 +3845,7 @@
       </c>
       <c r="H4" s="12">
         <f>COUNTIF(C3:C45,"No")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I4" s="16" t="s">
         <v>40</v>
@@ -3856,8 +3888,8 @@
       <c r="B6" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
+      <c r="C6" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -3868,8 +3900,8 @@
       <c r="B7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
+      <c r="C7" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="D7" s="3"/>
     </row>
@@ -3880,8 +3912,8 @@
       <c r="B8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>53</v>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -4381,7 +4413,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5028,8 +5060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5136,7 +5168,9 @@
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>123</v>
       </c>
@@ -5155,7 +5189,9 @@
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="29"/>
+      <c r="C6" s="23" t="s">
+        <v>128</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>123</v>
       </c>
@@ -5172,7 +5208,9 @@
       <c r="B7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="22" t="s">
+        <v>129</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>124</v>
       </c>
@@ -5191,7 +5229,9 @@
       <c r="B8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>130</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>123</v>
       </c>
@@ -5210,7 +5250,9 @@
       <c r="B9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>131</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
         <v>12</v>
@@ -5231,4 +5273,170 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="49.140625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="I3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>137</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6">
+      <formula1>$I$2:$I$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update sample tcs for TREEVIEW
</commit_message>
<xml_diff>
--- a/out/production/KeyWordDriven/testing/dataEngine/TestSuite1.xlsx
+++ b/out/production/KeyWordDriven/testing/dataEngine/TestSuite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="2" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="TestCase6" sheetId="8" r:id="rId7"/>
     <sheet name="TestCase7" sheetId="9" r:id="rId8"/>
     <sheet name="TestCase8" sheetId="10" r:id="rId9"/>
+    <sheet name="TestCase9" sheetId="11" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TestSuite!$G$21:$G$22</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="156">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -472,6 +473,33 @@
   </si>
   <si>
     <t>RDB_FEMALE</t>
+  </si>
+  <si>
+    <t>http://www.javascripttoolbox.com/lib/mktree/</t>
+  </si>
+  <si>
+    <t>TS_010</t>
+  </si>
+  <si>
+    <t>clickTreeViewItem</t>
+  </si>
+  <si>
+    <t>TREE_DEFAULT</t>
+  </si>
+  <si>
+    <t>config.txt</t>
+  </si>
+  <si>
+    <t>schedule.id</t>
+  </si>
+  <si>
+    <t>verifyTreeViewItemExist</t>
+  </si>
+  <si>
+    <t>verifyTreeViewItemNotExist</t>
+  </si>
+  <si>
+    <t>AAAAAAAAA</t>
   </si>
 </sst>
 </file>
@@ -1246,10 +1274,10 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3747,8 +3775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3840,7 +3868,7 @@
       </c>
       <c r="H3" s="12">
         <f>COUNTIF(C2:C44,"Yes")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I3" s="16" t="s">
         <v>41</v>
@@ -3880,7 +3908,7 @@
       </c>
       <c r="H4" s="12">
         <f>COUNTIF(C3:C45,"No")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I4" s="16" t="s">
         <v>40</v>
@@ -3971,8 +3999,8 @@
       <c r="B10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>53</v>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="D10" s="3"/>
     </row>
@@ -4000,6 +4028,193 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="49.140625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="I3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6">
+      <formula1>$I$2:$I$3</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5315,7 +5530,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:E24"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5478,10 +5693,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5670,7 +5885,7 @@
         <v>84</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="3" t="s">
         <v>146</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -5678,6 +5893,21 @@
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>